<commit_message>
If Else condition for devis or facture
</commit_message>
<xml_diff>
--- a/web/media/templates/dev-template.xlsx
+++ b/web/media/templates/dev-template.xlsx
@@ -140,6 +140,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,6 +161,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -167,6 +169,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -174,11 +177,13 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -186,12 +191,14 @@
       <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10.5"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -199,34 +206,40 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="7"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,15 +329,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -344,7 +357,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,7 +413,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,7 +425,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -424,7 +437,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,22 +453,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -471,9 +484,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>188280</xdr:colOff>
+      <xdr:colOff>187920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -487,7 +500,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="39600" y="0"/>
-          <a:ext cx="2891880" cy="717120"/>
+          <a:ext cx="2891520" cy="716760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -509,11 +522,11 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J30" activeCellId="0" sqref="J30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.84"/>
@@ -521,6 +534,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
modifying template and git ignore
</commit_message>
<xml_diff>
--- a/web/media/templates/dev-template.xlsx
+++ b/web/media/templates/dev-template.xlsx
@@ -469,12 +469,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -490,9 +490,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>187200</xdr:colOff>
+      <xdr:colOff>186840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>144720</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -506,7 +506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="39600" y="0"/>
-          <a:ext cx="2890800" cy="716040"/>
+          <a:ext cx="2890440" cy="715680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -528,11 +528,11 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.84"/>
@@ -540,7 +540,6 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,7 +762,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="18"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="H20" s="19" t="n">
+        <f aca="false">SUM(G20*F20)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16"/>
@@ -773,7 +775,10 @@
       <c r="E21" s="20"/>
       <c r="F21" s="21"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="22" t="n">
+        <f aca="false">SUM(G21*F21)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16"/>
@@ -783,7 +788,10 @@
       <c r="E22" s="20"/>
       <c r="F22" s="21"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="H22" s="22" t="n">
+        <f aca="false">SUM(G22*F22)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16"/>
@@ -793,7 +801,10 @@
       <c r="E23" s="20"/>
       <c r="F23" s="21"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
+      <c r="H23" s="22" t="n">
+        <f aca="false">SUM(G23*F23)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16"/>
@@ -803,7 +814,10 @@
       <c r="E24" s="20"/>
       <c r="F24" s="21"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="H24" s="22" t="n">
+        <f aca="false">SUM(G24*F24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16"/>
@@ -813,7 +827,10 @@
       <c r="E25" s="20"/>
       <c r="F25" s="21"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
+      <c r="H25" s="22" t="n">
+        <f aca="false">SUM(G25*F25)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16"/>
@@ -823,7 +840,10 @@
       <c r="E26" s="20"/>
       <c r="F26" s="21"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
+      <c r="H26" s="22" t="n">
+        <f aca="false">SUM(G26*F26)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16"/>
@@ -833,7 +853,10 @@
       <c r="E27" s="20"/>
       <c r="F27" s="21"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
+      <c r="H27" s="22" t="n">
+        <f aca="false">SUM(G27*F27)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16"/>
@@ -843,7 +866,10 @@
       <c r="E28" s="20"/>
       <c r="F28" s="21"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
+      <c r="H28" s="22" t="n">
+        <f aca="false">SUM(G28*F28)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16"/>
@@ -853,7 +879,10 @@
       <c r="E29" s="20"/>
       <c r="F29" s="21"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
+      <c r="H29" s="22" t="n">
+        <f aca="false">SUM(G29*F29)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="16"/>
@@ -863,7 +892,10 @@
       <c r="E30" s="20"/>
       <c r="F30" s="21"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
+      <c r="H30" s="22" t="n">
+        <f aca="false">SUM(G30*F30)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16"/>
@@ -873,7 +905,10 @@
       <c r="E31" s="20"/>
       <c r="F31" s="21"/>
       <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
+      <c r="H31" s="22" t="n">
+        <f aca="false">SUM(G31*F31)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="16"/>
@@ -883,7 +918,10 @@
       <c r="E32" s="20"/>
       <c r="F32" s="21"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
+      <c r="H32" s="22" t="n">
+        <f aca="false">SUM(G32*F32)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16"/>
@@ -893,7 +931,10 @@
       <c r="E33" s="20"/>
       <c r="F33" s="21"/>
       <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
+      <c r="H33" s="22" t="n">
+        <f aca="false">SUM(G33*F33)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16"/>
@@ -903,7 +944,10 @@
       <c r="E34" s="20"/>
       <c r="F34" s="21"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
+      <c r="H34" s="22" t="n">
+        <f aca="false">SUM(G34*F34)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16"/>
@@ -913,7 +957,10 @@
       <c r="E35" s="20"/>
       <c r="F35" s="21"/>
       <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
+      <c r="H35" s="22" t="n">
+        <f aca="false">SUM(G35*F35)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16"/>
@@ -923,7 +970,10 @@
       <c r="E36" s="20"/>
       <c r="F36" s="21"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
+      <c r="H36" s="22" t="n">
+        <f aca="false">SUM(G36*F36)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16"/>
@@ -933,7 +983,10 @@
       <c r="E37" s="20"/>
       <c r="F37" s="21"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
+      <c r="H37" s="22" t="n">
+        <f aca="false">SUM(G37*F37)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16"/>
@@ -943,7 +996,10 @@
       <c r="E38" s="20"/>
       <c r="F38" s="21"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
+      <c r="H38" s="22" t="n">
+        <f aca="false">SUM(G38*F38)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="23"/>
@@ -953,7 +1009,10 @@
       <c r="E39" s="24"/>
       <c r="F39" s="25"/>
       <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
+      <c r="H39" s="26" t="n">
+        <f aca="false">SUM(G39*F39)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">

</xml_diff>

<commit_message>
user email in spreadsheet
</commit_message>
<xml_diff>
--- a/web/media/templates/dev-template.xlsx
+++ b/web/media/templates/dev-template.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Fax : 01.60.71.62.32</t>
   </si>
   <si>
-    <t xml:space="preserve">E-mail : touchet@acces77.fr</t>
+    <t xml:space="preserve">E-mail : </t>
   </si>
   <si>
     <t xml:space="preserve">A l’attention de</t>
@@ -314,7 +314,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -347,6 +347,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -469,12 +473,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -490,9 +494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>186840</xdr:colOff>
+      <xdr:colOff>186480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -506,7 +510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="39600" y="0"/>
-          <a:ext cx="2890440" cy="715680"/>
+          <a:ext cx="2890080" cy="715320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -528,15 +532,16 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
@@ -649,14 +654,15 @@
       <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
@@ -668,16 +674,16 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
@@ -691,10 +697,10 @@
       <c r="G14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="10"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -711,355 +717,355 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19" t="n">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20" t="n">
         <f aca="false">SUM(G20*F20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22" t="n">
+      <c r="A21" s="17"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23" t="n">
         <f aca="false">SUM(G21*F21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22" t="n">
+      <c r="A22" s="17"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23" t="n">
         <f aca="false">SUM(G22*F22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22" t="n">
+      <c r="A23" s="17"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23" t="n">
         <f aca="false">SUM(G23*F23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22" t="n">
+      <c r="A24" s="17"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23" t="n">
         <f aca="false">SUM(G24*F24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22" t="n">
+      <c r="A25" s="17"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23" t="n">
         <f aca="false">SUM(G25*F25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22" t="n">
+      <c r="A26" s="17"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23" t="n">
         <f aca="false">SUM(G26*F26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22" t="n">
+      <c r="A27" s="17"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23" t="n">
         <f aca="false">SUM(G27*F27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22" t="n">
+      <c r="A28" s="17"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23" t="n">
         <f aca="false">SUM(G28*F28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22" t="n">
+      <c r="A29" s="17"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23" t="n">
         <f aca="false">SUM(G29*F29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22" t="n">
+      <c r="A30" s="17"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23" t="n">
         <f aca="false">SUM(G30*F30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22" t="n">
+      <c r="A31" s="17"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23" t="n">
         <f aca="false">SUM(G31*F31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22" t="n">
+      <c r="A32" s="17"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23" t="n">
         <f aca="false">SUM(G32*F32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22" t="n">
+      <c r="A33" s="17"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23" t="n">
         <f aca="false">SUM(G33*F33)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22" t="n">
+      <c r="A34" s="17"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23" t="n">
         <f aca="false">SUM(G34*F34)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="16"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22" t="n">
+      <c r="A35" s="17"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23" t="n">
         <f aca="false">SUM(G35*F35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22" t="n">
+      <c r="A36" s="17"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23" t="n">
         <f aca="false">SUM(G36*F36)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="16"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22" t="n">
+      <c r="A37" s="17"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23" t="n">
         <f aca="false">SUM(G37*F37)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="16"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22" t="n">
+      <c r="A38" s="17"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23" t="n">
         <f aca="false">SUM(G38*F38)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26" t="n">
+      <c r="A39" s="24"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27" t="n">
         <f aca="false">SUM(G39*F39)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="27" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="14" t="s">
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H40" s="28"/>
+      <c r="H40" s="29"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="30" t="s">
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="31" t="n">
+      <c r="H41" s="32" t="n">
         <f aca="false">SUM(H20:H40)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="14" t="s">
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H42" s="28" t="n">
+      <c r="H42" s="29" t="n">
         <f aca="false">SUM(H43-H41)</f>
         <v>0</v>
       </c>
@@ -1068,89 +1074,89 @@
       <c r="A43" s="0"/>
       <c r="B43" s="0"/>
       <c r="C43" s="0"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="30" t="s">
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H43" s="31" t="n">
+      <c r="H43" s="32" t="n">
         <f aca="false">SUM(H41*1.2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="33" t="s">
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="F45" s="34" t="s">
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="F45" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F46" s="35" t="s">
+      <c r="F46" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="37" t="s">
+      <c r="C50" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="37" t="s">
+      <c r="C51" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
     </row>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1159,7 +1165,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="52">
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A5:D5"/>
@@ -1170,8 +1176,9 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="A15:B15"/>

</xml_diff>

<commit_message>
add email in spreads
</commit_message>
<xml_diff>
--- a/web/media/templates/dev-template.xlsx
+++ b/web/media/templates/dev-template.xlsx
@@ -483,48 +483,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>39600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>186480</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="39600" y="0"/>
-          <a:ext cx="2890080" cy="715320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -545,6 +503,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,6 +1185,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add name on devis
</commit_message>
<xml_diff>
--- a/web/media/templates/dev-template.xlsx
+++ b/web/media/templates/dev-template.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Vos commandes peuvent nous être adressées par</t>
   </si>
   <si>
-    <t xml:space="preserve">Sincères salutations, Arnaud TOUCHET</t>
+    <t xml:space="preserve">Sincères salutations, </t>
   </si>
   <si>
     <t xml:space="preserve">mail à l'adresse figurant sur ce devis, ou télécopie</t>
@@ -490,8 +490,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,7 +503,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,7 +1170,7 @@
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A44:E44"/>
     <mergeCell ref="F44:H44"/>
-    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A45:B45"/>
     <mergeCell ref="F45:H45"/>
     <mergeCell ref="F46:H46"/>
     <mergeCell ref="A47:H47"/>

</xml_diff>